<commit_message>
feat: add emi to ind_constraint_co2eq row
</commit_message>
<xml_diff>
--- a/tests/test_data/test_structures/emission_constraint_example.xlsx
+++ b/tests/test_data/test_structures/emission_constraint_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxiao/Documents/code/ril/data_adapter/tests/test_data/test_structures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2C6FC8-5BA6-8048-9B70-A7A6975633C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C6ADFB-2F42-1F46-BCFA-79522EB8EA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Parameter_Input-Output" sheetId="2" r:id="rId2"/>
     <sheet name="Helper_Set" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="32">
   <si>
     <t>id</t>
   </si>
@@ -121,13 +121,17 @@
   </si>
   <si>
     <t>iip_heat_high,emi_co2_f_ind,emi_ch4_f_ind,emi_n2o_f_ind</t>
+  </si>
+  <si>
+    <t>ind_constraint_co2eq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -139,6 +143,11 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -161,8 +170,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -497,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -606,6 +618,14 @@
       </c>
       <c r="D7" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>